<commit_message>
test: Add test for manager roles and login
</commit_message>
<xml_diff>
--- a/media/advancePayment_1.xlsx
+++ b/media/advancePayment_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
tests: add testMain file with logic to run all unit tests with a single command
</commit_message>
<xml_diff>
--- a/media/advancePayment_1.xlsx
+++ b/media/advancePayment_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fix: add library to requirements.txt
</commit_message>
<xml_diff>
--- a/media/advancePayment_1.xlsx
+++ b/media/advancePayment_1.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>RAD123456</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>67890</t>
+          <t>OP12345</t>
         </is>
       </c>
       <c r="H6" s="3" t="n"/>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>45047</v>
+        <v>-692739</v>
       </c>
       <c r="H8" s="3" t="n"/>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="H9" s="3" t="n"/>
@@ -598,7 +598,7 @@
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>CC123</t>
         </is>
       </c>
       <c r="H10" s="3" t="n"/>
@@ -627,7 +627,7 @@
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Nueva York</t>
         </is>
       </c>
       <c r="H13" s="3" t="n"/>
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="C14" s="6" t="n">
-        <v>45061</v>
+        <v>-692739</v>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="F14" s="6" t="n">
-        <v>45066</v>
+        <v>-692739</v>
       </c>
       <c r="H14" s="3" t="n"/>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="C15" s="7" t="inlineStr">
         <is>
-          <t>Reunión de negocios</t>
+          <t>Asistir a una conferencia de ventas</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -675,7 +675,7 @@
       </c>
       <c r="C17" s="7" t="inlineStr">
         <is>
-          <t>PESOS COLOMBIANOS</t>
+          <t>DOLARES</t>
         </is>
       </c>
       <c r="H17" s="3" t="n"/>
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="E18" s="6" t="n">
-        <v>45060</v>
+        <v>-693530</v>
       </c>
       <c r="H18" s="3" t="n"/>
     </row>
@@ -705,23 +705,16 @@
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>Transporte</t>
+          <t>Alojamiento</t>
         </is>
       </c>
       <c r="E21" s="9" t="n">
-        <v>50000</v>
+        <v>500</v>
       </c>
       <c r="H21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Alojamiento</t>
-        </is>
-      </c>
-      <c r="E22" s="9" t="n">
-        <v>100000</v>
-      </c>
+      <c r="E22" s="9" t="n"/>
       <c r="H22" s="3" t="n"/>
     </row>
     <row r="23">
@@ -778,12 +771,12 @@
     <row r="33">
       <c r="B33" s="7" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="E33" s="7" t="inlineStr">
         <is>
-          <t>María Rodríguez</t>
+          <t>Jane Smith</t>
         </is>
       </c>
       <c r="H33" s="3" t="n"/>
@@ -807,12 +800,12 @@
     <row r="36">
       <c r="B36" s="7" t="inlineStr">
         <is>
-          <t>María Rodríguez</t>
+          <t>Jane Smith</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>María Rodríguez</t>
+          <t>Jane Smith</t>
         </is>
       </c>
       <c r="H36" s="3" t="n"/>

</xml_diff>